<commit_message>
2022.01.07 | Meng Haoyang | Solved Almost All The Bugs In T1 (V2.5).py, Left Error Catching Not Finished
</commit_message>
<xml_diff>
--- a/高发人员户籍.xlsx
+++ b/高发人员户籍.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>省份</t>
   </si>
@@ -124,106 +124,7 @@
     <t>澳门</t>
   </si>
   <si>
-    <t>err</t>
-  </si>
-  <si>
-    <t>237</t>
-  </si>
-  <si>
-    <t>230</t>
-  </si>
-  <si>
-    <t>213</t>
-  </si>
-  <si>
-    <t>204</t>
-  </si>
-  <si>
-    <t>202</t>
-  </si>
-  <si>
-    <t>190</t>
-  </si>
-  <si>
-    <t>186</t>
-  </si>
-  <si>
-    <t>169</t>
-  </si>
-  <si>
-    <t>159</t>
-  </si>
-  <si>
-    <t>158</t>
-  </si>
-  <si>
-    <t>149</t>
-  </si>
-  <si>
-    <t>147</t>
-  </si>
-  <si>
-    <t>144</t>
-  </si>
-  <si>
-    <t>143</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>131</t>
-  </si>
-  <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>129</t>
-  </si>
-  <si>
-    <t>126</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>92</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>-1.0</t>
   </si>
 </sst>
 </file>
@@ -436,7 +337,7 @@
                   <c:v>澳门</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>err</c:v>
+                  <c:v>-1.0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -550,7 +451,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -977,280 +878,280 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>37</v>
+      <c r="B2">
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>38</v>
+      <c r="B3">
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>39</v>
+      <c r="B4">
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>40</v>
+      <c r="B5">
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>41</v>
+      <c r="B6">
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>42</v>
+      <c r="B7">
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>43</v>
+      <c r="B8">
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>44</v>
+      <c r="B9">
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>45</v>
+      <c r="B10">
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>46</v>
+      <c r="B11">
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>47</v>
+      <c r="B12">
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>48</v>
+      <c r="B13">
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>48</v>
+      <c r="B14">
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
-        <v>49</v>
+      <c r="B15">
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
-        <v>50</v>
+      <c r="B16">
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
-        <v>51</v>
+      <c r="B17">
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
-        <v>52</v>
+      <c r="B18">
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
-        <v>53</v>
+      <c r="B19">
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
-        <v>54</v>
+      <c r="B20">
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
-        <v>55</v>
+      <c r="B21">
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
-        <v>56</v>
+      <c r="B22">
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
-        <v>57</v>
+      <c r="B23">
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
-        <v>58</v>
+      <c r="B24">
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
-        <v>59</v>
+      <c r="B25">
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
-        <v>60</v>
+      <c r="B26">
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="s">
-        <v>61</v>
+      <c r="B27">
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
-        <v>62</v>
+      <c r="B28">
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
-      <c r="B29" t="s">
-        <v>63</v>
+      <c r="B29">
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="s">
-        <v>64</v>
+      <c r="B30">
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
-      <c r="B31" t="s">
-        <v>65</v>
+      <c r="B31">
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
-        <v>66</v>
+      <c r="B32">
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
-        <v>67</v>
+      <c r="B33">
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="B34" t="s">
-        <v>68</v>
+      <c r="B34">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
-        <v>69</v>
+      <c r="B35">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B36" t="s">
-        <v>69</v>
+      <c r="B36">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>